<commit_message>
WIP - Admin Module
</commit_message>
<xml_diff>
--- a/docs/qa/matrices/admin-module.xlsx
+++ b/docs/qa/matrices/admin-module.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth\Documents\QA-Journey\CertifyHub-Tests\CertifyHub---Test-Strategy\docs\qa\matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB33F6E-91B2-4F6B-971B-E8AFB3EC5E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DA29DB-EBDE-4BCF-8B46-D575427DE4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B6A1F70D-DD27-4DBD-A810-A0A08D366CEF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>TEST CASE ID</t>
   </si>
@@ -180,7 +180,65 @@
 6. Click Generate and Send.</t>
   </si>
   <si>
-    <t>. Login as Admin.
+    <t>1. Login as Admin.
+2. Click signout.
+3. When the signout confirmation pops up click Ok.</t>
+  </si>
+  <si>
+    <t>1. Login as Admin.
+2. Click signout.
+3. When the signout confirmation pops up click Ok.
+4. Click the browsers back button to go back to the previous url.</t>
+  </si>
+  <si>
+    <t>TC28</t>
+  </si>
+  <si>
+    <t>Verify the Save Layout Blueprint does not reproduce again when its copy is already saved.</t>
+  </si>
+  <si>
+    <t>The app does not allow duplicate of design. (restrict resave of unmodified layout).</t>
+  </si>
+  <si>
+    <t>1. Login as Admin.
+2. Click "Templates" in the sidebar.
+3. Click "Reuse" your desired template.
+4. Click Save Layout Blueprint.</t>
+  </si>
+  <si>
+    <t>TC31</t>
+  </si>
+  <si>
+    <t>Verify the system does not allow txt files renamed as ".xsls"</t>
+  </si>
+  <si>
+    <t>The app does not allow ".txt" files.</t>
+  </si>
+  <si>
+    <t>1. Login as Admin. 
+2. Click "Templates" in the sidebar. 
+3. Click "Reuse" your desired template. 
+4. Upload text file renamed as ".xsls"</t>
+  </si>
+  <si>
+    <t>TC34</t>
+  </si>
+  <si>
+    <t>Verify system behavior when admin upload's corrupted file.</t>
+  </si>
+  <si>
+    <t>The app blocks the request because of the corrupted file.</t>
+  </si>
+  <si>
+    <t>1. Login as Admin. 
+2. Click "Templates" in the sidebar. 
+3. Click "Reuse" your desired template. 
+4. Upload corrupted excel file. 
+5. Enable send Certificates. 
+6. Click Generate and Send.</t>
+  </si>
+  <si>
+    <t>1. Login as Admin.
 2. Click "Templates" in the sidebar.
 3. Click "Reuse" your desired template.
 4. Upload excel file containing the really long string of name.
@@ -188,30 +246,71 @@
 6. Click Generate and Send.</t>
   </si>
   <si>
-    <t>1. Login as Admin.
-2. Click signout.
-3. When the signout confirmation pops up click Ok.</t>
-  </si>
-  <si>
-    <t>1. Login as Admin.
-2. Click signout.
-3. When the signout confirmation pops up click Ok.
-4. Click the browsers back button to go back to the previous url.</t>
-  </si>
-  <si>
-    <t>TC28</t>
-  </si>
-  <si>
-    <t>Verify the Save Layout Blueprint does not reproduce again when its copy is already saved.</t>
-  </si>
-  <si>
-    <t>The app does not allow duplicate of design. (restrict resave of unmodified layout).</t>
-  </si>
-  <si>
-    <t>1. Login as Admin.
-2. Click "Templates" in the sidebar.
-3. Click "Reuse" your desired template.
-4. Click Save Layout Blueprint.</t>
+    <t>TC35</t>
+  </si>
+  <si>
+    <t>Verify sytem behavior when Admin uploads an oversized excel file.</t>
+  </si>
+  <si>
+    <t>The app blocks the request due to file size limit being hit.</t>
+  </si>
+  <si>
+    <t>1. Login as Admin. 
+2. Click "Templates" in the sidebar. 
+3. Click "Reuse" your desired template. 
+4. Upload really large sized excel file. 
+5. Enable send Certificates. 
+6. Click Generate and Send.</t>
+  </si>
+  <si>
+    <t>TC36</t>
+  </si>
+  <si>
+    <t>Verify system behavior when 1 of 10 individuals is missing an email.</t>
+  </si>
+  <si>
+    <t>The app sends the certificate to 9 individuals.</t>
+  </si>
+  <si>
+    <t>1. Login as Admin. 
+2. Click "Templates" in the sidebar. 
+3. Click "Reuse" your desired template. 
+4. Upload the excel file containing the needed credentials of 10 people and 1 of them is missing an email. 
+5. Enable send Certificates. 
+6. Click Generate and Send.</t>
+  </si>
+  <si>
+    <t>TC37</t>
+  </si>
+  <si>
+    <t>Verify system behavior when 2 admins generate a certificate (separate browser window).</t>
+  </si>
+  <si>
+    <t>The app allows only one admin access.</t>
+  </si>
+  <si>
+    <t>1. Login as Admin. (2 browser simultaneously doing this) 
+2. Click "Templates" in the sidebar. (2 browser simultaneously doing this) 
+3. Click "Reuse" your desired template. (2 browser simultaneously doing this) 
+4. Upload excel file containing the certificate reciever's appropriate data (Name, Email). (2 browser simultaneously doing this) 
+5. Enable send Certificates. (2 browser simultaneously doing this) 
+6. Click Generate and Send. (2 browser simultaneously doing this)</t>
+  </si>
+  <si>
+    <t>TC38</t>
+  </si>
+  <si>
+    <t>Verify system behavior when an excel file is named as an emoji.</t>
+  </si>
+  <si>
+    <t>The app allows the upload request.</t>
+  </si>
+  <si>
+    <t>1. Login as Admin. 
+2. Click "Templates" in the sidebar. 
+3. Click "Reuse" your desired template. 
+4. Upload excel file having the file name "😊" 5. Enable send Certificates. 
+6. Click Generate and Send.</t>
   </si>
 </sst>
 </file>
@@ -289,18 +388,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -328,8 +416,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>304937</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="3" name="Ink 2">
@@ -348,7 +436,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="3" name="Ink 2">
@@ -727,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E1D032-4572-4826-B4CD-3DD8E0382E83}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -921,7 +1009,7 @@
         <v>26</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>27</v>
@@ -947,7 +1035,7 @@
         <v>29</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>30</v>
@@ -973,7 +1061,7 @@
         <v>32</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>33</v>
@@ -982,24 +1070,139 @@
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:6" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="3" t="s">
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:6" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>44</v>
+      <c r="B20" s="3"/>
+      <c r="C20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:6" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:6" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:6" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:6" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:6" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>